<commit_message>
fix: enhance COM object cleanup and resource management in Win32 PowerPoint conversion to prevent residual processes.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <t>销售额</t>
   </si>
   <si>
-    <t>基金产品名称</t>
+    <t>基金名称</t>
   </si>
   <si>
     <t>数据日期</t>
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="4"/>

</xml_diff>